<commit_message>
done validation add user
</commit_message>
<xml_diff>
--- a/Data Files/Delete Employees Excel (Single).xlsx
+++ b/Data Files/Delete Employees Excel (Single).xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afaa1\Katalon Studio\PROJECT-WEB.git\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406E9F01-9932-4798-9BFC-54E8B259B157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9F832606-ED90-42DD-B361-25CF34E4AAC9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -60,7 +60,28 @@
     <t>Existing Username</t>
   </si>
   <si>
-    <t>Chen130133</t>
+    <t>Chen153954</t>
+  </si>
+  <si>
+    <t>Chen154309</t>
+  </si>
+  <si>
+    <t>Chen154711</t>
+  </si>
+  <si>
+    <t>Chen155002</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Chen160806</t>
+  </si>
+  <si>
+    <t>Chen161112</t>
+  </si>
+  <si>
+    <t>Chen161320</t>
   </si>
 </sst>
 </file>
@@ -97,17 +118,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -124,10 +145,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -162,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -197,7 +218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -291,21 +312,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -322,7 +343,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -374,26 +395,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -406,22 +428,22 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">Sheet2!$A2</f>
-        <v>Chen130151</v>
+        <v>Chen154122</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675635E1-F48E-47EE-AEC8-E07E2AF05348}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675635E1-F48E-47EE-AEC8-E07E2AF05348}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -429,10 +451,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -452,38 +474,38 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">B2&amp;C2</f>
-        <v>Chen130151</v>
+        <v>Chen154122</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">TEXT(D2,"hhmmss")</f>
-        <v>130151</v>
+        <v>154122</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">NOW()</f>
-        <v>44872.542949537034</v>
+        <v>44872.653723611111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f ca="1">B3&amp;C3</f>
-        <v>Ehi130151</v>
+        <v>Ehi154122</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="str">
         <f ca="1">TEXT(D3,"hhmmss")</f>
-        <v>130151</v>
+        <v>154122</v>
       </c>
       <c r="D3" s="1">
         <f ca="1">NOW()</f>
-        <v>44872.542949537034</v>
+        <v>44872.653723611111</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>